<commit_message>
IconProto추가, CookieProto에 Sprite 추가, CookiePopup 작업중
</commit_message>
<xml_diff>
--- a/Data/Excel/Proto/Cookie.xlsx
+++ b/Data/Excel/Proto/Cookie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA65E4F7-0339-4A3A-ABDD-34244518ADC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB107E98-F019-4C67-9D04-2ABBFC73F7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A122D7ED-2698-4919-AFB3-8D3D98F98776}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Num</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>InitSoulStone</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cookie/DummyCookie1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1109,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44314A49-C27D-4F35-AB30-B78979822F33}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1134,7 @@
     <col min="4" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1165,11 @@
       <c r="J1" t="s">
         <v>33</v>
       </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1185,8 +1200,11 @@
       <c r="J2" t="s">
         <v>34</v>
       </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1010</v>
       </c>
@@ -1217,8 +1235,11 @@
       <c r="J3">
         <v>1</v>
       </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1020</v>
       </c>
@@ -1249,8 +1270,11 @@
       <c r="J4">
         <v>2</v>
       </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -1281,8 +1305,11 @@
       <c r="J5">
         <v>5</v>
       </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3010</v>
       </c>
@@ -1313,8 +1340,11 @@
       <c r="J6">
         <v>1</v>
       </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4010</v>
       </c>
@@ -1345,8 +1375,11 @@
       <c r="J7">
         <v>10</v>
       </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5010</v>
       </c>
@@ -1377,8 +1410,11 @@
       <c r="J8">
         <v>10</v>
       </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6010</v>
       </c>
@@ -1409,8 +1445,11 @@
       <c r="J9">
         <v>21</v>
       </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6020</v>
       </c>
@@ -1440,6 +1479,9 @@
       </c>
       <c r="J10">
         <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>